<commit_message>
Added documentation on instruction set
</commit_message>
<xml_diff>
--- a/005d_InstructionSet.xlsx
+++ b/005d_InstructionSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\athens\logisim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F7FC4F-E9B3-4297-9E2E-9BE37DF395B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53176EFE-59BE-4D14-8FD8-E1D515DA796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7335" yWindow="1785" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Functions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Value</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Do nothing</t>
   </si>
   <si>
-    <t>Load to Write Addr</t>
-  </si>
-  <si>
     <t>0x0</t>
   </si>
   <si>
@@ -273,13 +270,58 @@
     <t>PUSH</t>
   </si>
   <si>
-    <t>Pop</t>
-  </si>
-  <si>
     <t>JZ</t>
   </si>
   <si>
     <t>Jump</t>
+  </si>
+  <si>
+    <t>Print to TTY</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>Unconditional jump</t>
+  </si>
+  <si>
+    <t>Conditional jump</t>
+  </si>
+  <si>
+    <t>Add number and save to Write Addr</t>
+  </si>
+  <si>
+    <t>Inverse bits and save to Write Addr</t>
+  </si>
+  <si>
+    <t>Subtract number and save to Write Addr</t>
+  </si>
+  <si>
+    <t>OR number and save to Write Addr</t>
+  </si>
+  <si>
+    <t>AND number and save to Write Addr</t>
+  </si>
+  <si>
+    <t>XOR number and save to Write Addr</t>
+  </si>
+  <si>
+    <t>Pop data from stack</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>Load from Reg to Write Addr</t>
+  </si>
+  <si>
+    <t>Load constant to Write Addr</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,10 +1253,10 @@
         <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1305,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>62</v>
@@ -1313,7 +1355,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>64</v>
@@ -1342,7 +1384,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>63</v>
@@ -1366,12 +1408,15 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>31</v>
@@ -1391,11 +1436,16 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -1415,11 +1465,16 @@
       <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -1439,11 +1494,16 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>38</v>
@@ -1463,11 +1523,16 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>39</v>
@@ -1487,11 +1552,16 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
@@ -1511,11 +1581,16 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -1535,11 +1610,16 @@
       <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -1559,11 +1639,13 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -1586,11 +1668,16 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
@@ -1611,15 +1698,15 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>44</v>
@@ -1645,7 +1732,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>45</v>
@@ -1665,7 +1755,9 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>